<commit_message>
Tables: adding in new table with cumulative proportions
</commit_message>
<xml_diff>
--- a/Tables/Table for project.xlsx
+++ b/Tables/Table for project.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
   <si>
     <t>Frequency of PE</t>
   </si>
@@ -251,6 +252,54 @@
   </si>
   <si>
     <t>Proportion of Correct Perceptions Across PE Freq.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>(0.0006)</t>
+  </si>
+  <si>
+    <t>(0.0052)</t>
+  </si>
+  <si>
+    <t>(0.0134)</t>
+  </si>
+  <si>
+    <t>(0.0177)</t>
+  </si>
+  <si>
+    <t>(0.0115)</t>
+  </si>
+  <si>
+    <t>(0.0145)</t>
+  </si>
+  <si>
+    <t>(0.0025)</t>
+  </si>
+  <si>
+    <t>(0.0074)</t>
+  </si>
+  <si>
+    <t>(0.0073)</t>
+  </si>
+  <si>
+    <t>(0.0031)</t>
+  </si>
+  <si>
+    <t>(0.0123)</t>
+  </si>
+  <si>
+    <t>(0.0316)</t>
+  </si>
+  <si>
+    <t>(0.0282)</t>
+  </si>
+  <si>
+    <t>(0.0071)</t>
+  </si>
+  <si>
+    <t>(0.0190)</t>
   </si>
 </sst>
 </file>
@@ -324,7 +373,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,8 +392,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -612,8 +667,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -653,8 +775,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -788,8 +932,44 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -809,6 +989,17 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -828,57 +1019,20 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF58BDFD"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1005,20 +1159,68 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF58BDFD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E14" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
   <autoFilter ref="A1:E14"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Frequency of PE" dataDxfId="8"/>
-    <tableColumn id="2" name="Underweight" dataDxfId="7"/>
-    <tableColumn id="3" name="Normal Weight" dataDxfId="6"/>
-    <tableColumn id="4" name="Overweight" dataDxfId="5"/>
-    <tableColumn id="5" name="Obese" dataDxfId="4"/>
+    <tableColumn id="1" name="Frequency of PE" dataDxfId="4"/>
+    <tableColumn id="2" name="Underweight" dataDxfId="3"/>
+    <tableColumn id="3" name="Normal Weight" dataDxfId="2"/>
+    <tableColumn id="4" name="Overweight" dataDxfId="1"/>
+    <tableColumn id="5" name="Obese" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1348,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:E14"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1643,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="N15" sqref="A1:N15"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2229,7 +2431,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="K13" s="21">
-        <v>0</v>
+        <v>5.5999999999999995E-4</v>
       </c>
       <c r="L13" s="21">
         <v>4.922E-2</v>
@@ -2272,7 +2474,7 @@
         <v>68</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="L14" s="33" t="s">
         <v>46</v>
@@ -2337,4 +2539,264 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" thickBot="1">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="45">
+        <v>0</v>
+      </c>
+      <c r="B2" s="52">
+        <v>9.8300000000000002E-3</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.10247000000000001</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3.5369999999999999E-2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>4.3679999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" thickBot="1">
+      <c r="A3" s="46"/>
+      <c r="B3" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="45">
+        <v>1</v>
+      </c>
+      <c r="B4" s="53">
+        <v>6.7000000000000002E-4</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.4070000000000003E-2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2.3700000000000001E-3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" thickBot="1">
+      <c r="A5" s="46"/>
+      <c r="B5" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="45">
+        <v>2</v>
+      </c>
+      <c r="B6" s="53">
+        <v>5.3099999999999996E-3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5.4269999999999999E-2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1.277E-2</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" thickBot="1">
+      <c r="A7" s="46"/>
+      <c r="B7" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="45">
+        <v>3</v>
+      </c>
+      <c r="B8" s="53">
+        <v>6.8500000000000002E-3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.15075</v>
+      </c>
+      <c r="D8" s="8">
+        <v>5.3069999999999999E-2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.0439999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" thickBot="1">
+      <c r="A9" s="46"/>
+      <c r="B9" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="45">
+        <v>4</v>
+      </c>
+      <c r="B10" s="49">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2.0310000000000002E-2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>4.5300000000000002E-3</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4.4299999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" thickBot="1">
+      <c r="A11" s="46"/>
+      <c r="B11" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="45">
+        <v>5</v>
+      </c>
+      <c r="B12" s="50">
+        <v>3.7699999999999999E-3</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.23763999999999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>6.5839999999999996E-2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>9.5649999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" thickBot="1">
+      <c r="A13" s="46"/>
+      <c r="B13" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="51">
+        <f xml:space="preserve"> B2+B4+B6+B8+B10+B12</f>
+        <v>2.6429999999999999E-2</v>
+      </c>
+      <c r="C14" s="51">
+        <f t="shared" ref="C14:E14" si="0" xml:space="preserve"> C2+C4+C6+C8+C10+C12</f>
+        <v>0.59950999999999999</v>
+      </c>
+      <c r="D14" s="51">
+        <f t="shared" si="0"/>
+        <v>0.17394999999999999</v>
+      </c>
+      <c r="E14" s="51">
+        <f t="shared" si="0"/>
+        <v>0.2001</v>
+      </c>
+      <c r="F14" s="54"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tables: labeling sheet names
</commit_message>
<xml_diff>
--- a/Tables/Table for project.xlsx
+++ b/Tables/Table for project.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table1-Prop_wt per Freq" sheetId="1" r:id="rId1"/>
+    <sheet name="Table2 Actual BMI vs perception" sheetId="2" r:id="rId2"/>
+    <sheet name="Table3-Proportion of Wt&amp;Freq" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -1550,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E6"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1845,7 +1845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tables: making more tables for the report due to more analysis
</commit_message>
<xml_diff>
--- a/Tables/Table for project.xlsx
+++ b/Tables/Table for project.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Table1-Prop_wt per Freq" sheetId="1" r:id="rId1"/>
     <sheet name="Table2 Actual BMI vs perception" sheetId="2" r:id="rId2"/>
     <sheet name="Table3-Proportion of Wt&amp;Freq" sheetId="3" r:id="rId3"/>
+    <sheet name="Table 4 - Enjoyment of PE" sheetId="4" r:id="rId4"/>
+    <sheet name="Table 5 - Correct Perc &amp; FreqPE" sheetId="5" r:id="rId5"/>
+    <sheet name="Table 6 -Correct Perc &amp; Enjoy " sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
   <si>
     <t>Frequency of PE</t>
   </si>
@@ -300,6 +303,87 @@
   </si>
   <si>
     <t>(0.0190)</t>
+  </si>
+  <si>
+    <t>agree</t>
+  </si>
+  <si>
+    <t>disagree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neither agree </t>
+  </si>
+  <si>
+    <t>nor disagree</t>
+  </si>
+  <si>
+    <t>strongly agree</t>
+  </si>
+  <si>
+    <t>strongly disagree</t>
+  </si>
+  <si>
+    <t>unsure</t>
+  </si>
+  <si>
+    <t>strongly</t>
+  </si>
+  <si>
+    <t>(0.0188)</t>
+  </si>
+  <si>
+    <t>(0.0089)</t>
+  </si>
+  <si>
+    <t>(0.0045)</t>
+  </si>
+  <si>
+    <t>(0.0241)</t>
+  </si>
+  <si>
+    <t>(0.0011)</t>
+  </si>
+  <si>
+    <t>(0.0194)</t>
+  </si>
+  <si>
+    <t>(0.0067)</t>
+  </si>
+  <si>
+    <t>(0.0079)</t>
+  </si>
+  <si>
+    <t>(0.0117)</t>
+  </si>
+  <si>
+    <t>(0.0065)</t>
+  </si>
+  <si>
+    <t>(0.0049)</t>
+  </si>
+  <si>
+    <t>(0.0033)</t>
+  </si>
+  <si>
+    <t>(0.0042)</t>
+  </si>
+  <si>
+    <t>Proportion of Each Response</t>
+  </si>
+  <si>
+    <t>False Perception</t>
+  </si>
+  <si>
+    <t>Correct Perception</t>
+  </si>
+  <si>
+    <t>Make Up in Population</t>
+  </si>
+  <si>
+    <t>Enjoy PE?</t>
+  </si>
+  <si>
+    <t>neither agree nor diagree</t>
   </si>
 </sst>
 </file>
@@ -373,7 +457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,8 +482,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -734,8 +836,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -797,8 +914,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -968,8 +1107,44 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1000,6 +1175,17 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1030,6 +1216,17 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -1551,7 +1748,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B2" sqref="B2:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1845,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2799,4 +2996,588 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="46" thickBot="1">
+      <c r="A1" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.27078000000000002</v>
+      </c>
+      <c r="D2" s="8">
+        <v>7.2749999999999995E-2</v>
+      </c>
+      <c r="E2" s="60">
+        <v>0.10032000000000001</v>
+      </c>
+      <c r="F2" s="8">
+        <f>B2+C2+D2+E2</f>
+        <v>0.45885000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" thickBot="1">
+      <c r="A3" s="46"/>
+      <c r="B3" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.252E-2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1.8489999999999999E-2</v>
+      </c>
+      <c r="E4" s="60">
+        <v>1.269E-2</v>
+      </c>
+      <c r="F4" s="8">
+        <f>B4+C4+D4+E4</f>
+        <v>6.3700000000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" thickBot="1">
+      <c r="A5" s="46"/>
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2.7310000000000001E-2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4.7099999999999998E-3</v>
+      </c>
+      <c r="E6" s="60">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="F6" s="8">
+        <f>B6+C6+D6+E6</f>
+        <v>4.9169999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" thickBot="1">
+      <c r="A7" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7.0699999999999999E-3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.26255000000000001</v>
+      </c>
+      <c r="D8" s="8">
+        <v>7.4050000000000005E-2</v>
+      </c>
+      <c r="E8" s="60">
+        <v>6.905E-2</v>
+      </c>
+      <c r="F8" s="8">
+        <f>B8+C8+D8+E8</f>
+        <v>0.41272000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" thickBot="1">
+      <c r="A9" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>5.2399999999999999E-3</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3.9500000000000004E-3</v>
+      </c>
+      <c r="E10" s="60">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F10" s="8">
+        <f>B10+C10+D10+E10</f>
+        <v>1.009E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" thickBot="1">
+      <c r="A11" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="8">
+        <v>4.3600000000000002E-3</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.1100000000000001E-3</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="62">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <f>B12+C12+D12+E12</f>
+        <v>5.47E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" thickBot="1">
+      <c r="A13" s="46"/>
+      <c r="B13" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="47"/>
+      <c r="B14" s="37">
+        <f>B2+B4+B6+B8+B10+B12</f>
+        <v>2.6429999999999999E-2</v>
+      </c>
+      <c r="C14" s="37">
+        <f t="shared" ref="C14:E14" si="0">C2+C4+C6+C8+C10+C12</f>
+        <v>0.5995100000000001</v>
+      </c>
+      <c r="D14" s="37">
+        <f t="shared" si="0"/>
+        <v>0.17394999999999999</v>
+      </c>
+      <c r="E14" s="63">
+        <f t="shared" si="0"/>
+        <v>0.20011000000000001</v>
+      </c>
+      <c r="F14" s="64">
+        <f>B14+C14+D14+E14</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31" thickBot="1">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="45">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>5.0209999999999998E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.14115</v>
+      </c>
+      <c r="D2" s="8">
+        <f>SUM(B2:C2)</f>
+        <v>0.19136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="45">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1.089E-2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>3.2509999999999997E-2</v>
+      </c>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D7" si="0">SUM(B3:C3)</f>
+        <v>4.3399999999999994E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="45">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2.5479999999999999E-2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>6.6479999999999997E-2</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>9.196E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="45">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>5.9630000000000002E-2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.18148</v>
+      </c>
+      <c r="D5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.24110999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="45">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2.511E-2</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>2.9270000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="A7" s="45">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.13772000000000001</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.26518000000000003</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.40290000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="47"/>
+      <c r="B8" s="37">
+        <f>SUM(B2,B3,B4,B5,B6,B7)</f>
+        <v>0.28809000000000001</v>
+      </c>
+      <c r="C8" s="37">
+        <f>SUM(C2,C3,C4,C5,C6,C7)</f>
+        <v>0.71191000000000004</v>
+      </c>
+      <c r="D8" s="37">
+        <f>SUM(B8:C8)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection sqref="A1:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31" thickBot="1">
+      <c r="A1" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.12313</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.33572999999999997</v>
+      </c>
+      <c r="D2" s="8">
+        <f>SUM(B2:C2)</f>
+        <v>0.45885999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2.325E-2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>4.045E-2</v>
+      </c>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D7" si="0">SUM(B3:C3)</f>
+        <v>6.3700000000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30">
+      <c r="A4" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.0919999999999999E-2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.8249999999999999E-2</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>4.9169999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.12396</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.28876000000000002</v>
+      </c>
+      <c r="D5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.41272000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2.48E-3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>1.008E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="A7" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="8">
+        <v>4.3600000000000002E-3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1.1100000000000001E-3</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>5.47E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="47"/>
+      <c r="B8" s="37">
+        <f>SUM(B2:B7)</f>
+        <v>0.28809999999999997</v>
+      </c>
+      <c r="C8" s="37">
+        <f>SUM(C2:C7)</f>
+        <v>0.71190000000000009</v>
+      </c>
+      <c r="D8" s="37">
+        <f>SUM(B8:C8)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>